<commit_message>
Edit the QA table
</commit_message>
<xml_diff>
--- a/documentation/QA.xlsx
+++ b/documentation/QA.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6E63CA1-032B-4E2B-A123-6E372DCBF0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nkk81\OneDrive\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3A58F87-0651-4022-8AE7-1F01C66D2934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Function Name</t>
   </si>
@@ -45,15 +37,9 @@
     <t>Actual result</t>
   </si>
   <si>
-    <t>decimalToBinary</t>
-  </si>
-  <si>
     <t>Converts decimal numbers to binary</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Convert decimal number to binary</t>
   </si>
   <si>
@@ -103,13 +89,28 @@
   </si>
   <si>
     <t>Assigns random values to two number variables</t>
+  </si>
+  <si>
+    <t>binaryToDecimal</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>userAnswer</t>
+  </si>
+  <si>
+    <t>Prompts the player for an answer</t>
+  </si>
+  <si>
+    <t>If the answer is wrong, asks the user for a new answer, otherwise stops the program</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,22 +476,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="44.140625" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="5" width="43" customWidth="1"/>
+    <col min="4" max="4" width="75" customWidth="1"/>
+    <col min="5" max="5" width="74.85546875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" customHeight="1">
+    <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -498,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -507,123 +509,140 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20.25" customHeight="1">
+    <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>